<commit_message>
to do list app
</commit_message>
<xml_diff>
--- a/requiment/001_todo_list.xlsx
+++ b/requiment/001_todo_list.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\training.tts\Training-html-css\requiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training-html-css\requiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF07AE4-7C6A-4374-816B-E1AB6497950E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADBB4FD-1582-4F79-9E3E-7D96D7F4C0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -59,7 +70,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -70,7 +81,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -94,7 +105,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -113,7 +124,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -132,7 +143,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -143,7 +154,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -165,7 +176,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -176,7 +187,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -192,7 +203,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -203,7 +214,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -219,7 +230,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -230,7 +241,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -246,7 +257,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -257,7 +268,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -273,7 +284,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -284,7 +295,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -295,7 +306,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -306,7 +317,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -343,7 +354,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -354,7 +365,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -370,7 +381,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -381,7 +392,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -400,7 +411,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -416,7 +427,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -427,7 +438,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -446,7 +457,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -465,7 +476,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -484,7 +495,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -503,7 +514,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -548,7 +559,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -567,7 +578,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -586,7 +597,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -610,7 +621,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -634,7 +645,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -654,7 +665,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -675,7 +686,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -693,7 +704,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -701,7 +712,7 @@
       <b/>
       <sz val="24"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -710,7 +721,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -719,7 +730,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -732,7 +743,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -740,7 +751,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1081,18 +1092,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2" ht="39.75">
+    <row r="1" spans="2:2" ht="31.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:2" ht="30">
+    <row r="2" spans="2:2" ht="23.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1112,7 +1123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="30">
+    <row r="6" spans="2:2" ht="23.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1182,7 +1193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="30">
+    <row r="20" spans="2:2" ht="23.25">
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1217,7 +1228,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:2">
+    <row r="27" spans="2:2" ht="16.5">
       <c r="B27" s="5" t="s">
         <v>38</v>
       </c>
@@ -1237,7 +1248,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="30">
+    <row r="31" spans="2:2" ht="23.25">
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
@@ -1267,7 +1278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="30">
+    <row r="37" spans="2:2" ht="23.25">
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>

</xml_diff>